<commit_message>
setup of config.yaml completed
</commit_message>
<xml_diff>
--- a/user_data1.xlsx
+++ b/user_data1.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -491,6 +491,18 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ankir</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>